<commit_message>
Trimmed out reliance on precalculated stats
Version 2 of the dice fairness estimator generates the stats without the bias vector or sphere fitting, and it's fast enough to do the simulated rolls live for each input dataset.
</commit_message>
<xml_diff>
--- a/Dice_test.xlsx
+++ b/Dice_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmullens/Documents/DnD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmullens/Documents/GitHub/Dice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B242C6-38C0-9448-9435-105AE9EF494E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D09874-4181-A144-97D9-911152B248FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{D71FB28A-5275-6641-8EEB-6B08F00334B6}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{D71FB28A-5275-6641-8EEB-6B08F00334B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Actually_test_d20s" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +42,7 @@
     <t>Blue:</t>
   </si>
   <si>
-    <t>(Rolling on the flat desk, pick up and reroll with minimal shaking most of the time)</t>
+    <t>(Rolling on the flat wood desk, pick up and reroll after some shaking, avoid bumping into things near end of roll)</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0194933F-D8D3-DD40-9924-A4C1D50508BE}">
-  <dimension ref="A1:F1001"/>
+  <dimension ref="A1:F1556"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A980" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1557" sqref="A1557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8562,6 +8566,4446 @@
         <v>10.5</v>
       </c>
     </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1002">
+        <v>19</v>
+      </c>
+      <c r="B1002">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1003">
+        <v>12</v>
+      </c>
+      <c r="B1003">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1004">
+        <v>20</v>
+      </c>
+      <c r="B1004">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1005">
+        <v>9</v>
+      </c>
+      <c r="B1005">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1006">
+        <v>10</v>
+      </c>
+      <c r="B1006">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1007">
+        <v>4</v>
+      </c>
+      <c r="B1007">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1008">
+        <v>13</v>
+      </c>
+      <c r="B1008">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1009">
+        <v>16</v>
+      </c>
+      <c r="B1009">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1010">
+        <v>19</v>
+      </c>
+      <c r="B1010">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1011">
+        <v>14</v>
+      </c>
+      <c r="B1011">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1012">
+        <v>13</v>
+      </c>
+      <c r="B1012">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1013">
+        <v>19</v>
+      </c>
+      <c r="B1013">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1014">
+        <v>11</v>
+      </c>
+      <c r="B1014">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1015">
+        <v>11</v>
+      </c>
+      <c r="B1015">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1016">
+        <v>9</v>
+      </c>
+      <c r="B1016">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1017">
+        <v>4</v>
+      </c>
+      <c r="B1017">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1018">
+        <v>10</v>
+      </c>
+      <c r="B1018">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1019">
+        <v>1</v>
+      </c>
+      <c r="B1019">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1020">
+        <v>11</v>
+      </c>
+      <c r="B1020">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1021">
+        <v>9</v>
+      </c>
+      <c r="B1021">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1022">
+        <v>15</v>
+      </c>
+      <c r="B1022">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1023">
+        <v>19</v>
+      </c>
+      <c r="B1023">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1024">
+        <v>5</v>
+      </c>
+      <c r="B1024">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1025">
+        <v>4</v>
+      </c>
+      <c r="B1025">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1026">
+        <v>13</v>
+      </c>
+      <c r="B1026">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1027">
+        <v>9</v>
+      </c>
+      <c r="B1027">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1028">
+        <v>4</v>
+      </c>
+      <c r="B1028">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1029">
+        <v>15</v>
+      </c>
+      <c r="B1029">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1030">
+        <v>16</v>
+      </c>
+      <c r="B1030">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1031">
+        <v>15</v>
+      </c>
+      <c r="B1031">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1032">
+        <v>13</v>
+      </c>
+      <c r="B1032">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1033">
+        <v>16</v>
+      </c>
+      <c r="B1033">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1034">
+        <v>4</v>
+      </c>
+      <c r="B1034">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1035">
+        <v>1</v>
+      </c>
+      <c r="B1035">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1036">
+        <v>1</v>
+      </c>
+      <c r="B1036">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1037">
+        <v>9</v>
+      </c>
+      <c r="B1037">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1038">
+        <v>2</v>
+      </c>
+      <c r="B1038">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1039">
+        <v>8</v>
+      </c>
+      <c r="B1039">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1040">
+        <v>14</v>
+      </c>
+      <c r="B1040">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1041">
+        <v>10</v>
+      </c>
+      <c r="B1041">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1042">
+        <v>3</v>
+      </c>
+      <c r="B1042">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1043">
+        <v>1</v>
+      </c>
+      <c r="B1043">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1044">
+        <v>4</v>
+      </c>
+      <c r="B1044">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1045">
+        <v>18</v>
+      </c>
+      <c r="B1045">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1046">
+        <v>16</v>
+      </c>
+      <c r="B1046">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1047">
+        <v>8</v>
+      </c>
+      <c r="B1047">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1048">
+        <v>13</v>
+      </c>
+      <c r="B1048">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1049">
+        <v>17</v>
+      </c>
+      <c r="B1049">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1050">
+        <v>10</v>
+      </c>
+      <c r="B1050">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1051">
+        <v>20</v>
+      </c>
+      <c r="B1051">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1052">
+        <v>7</v>
+      </c>
+      <c r="B1052">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1053">
+        <v>14</v>
+      </c>
+      <c r="B1053">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1054">
+        <v>9</v>
+      </c>
+      <c r="B1054">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1055">
+        <v>16</v>
+      </c>
+      <c r="B1055">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1056">
+        <v>11</v>
+      </c>
+      <c r="B1056">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1057">
+        <v>16</v>
+      </c>
+      <c r="B1057">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1058">
+        <v>13</v>
+      </c>
+      <c r="B1058">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1059">
+        <v>20</v>
+      </c>
+      <c r="B1059">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1060">
+        <v>19</v>
+      </c>
+      <c r="B1060">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1061">
+        <v>8</v>
+      </c>
+      <c r="B1061">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1062">
+        <v>16</v>
+      </c>
+      <c r="B1062">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1063">
+        <v>18</v>
+      </c>
+      <c r="B1063">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1064">
+        <v>10</v>
+      </c>
+      <c r="B1064">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1065">
+        <v>5</v>
+      </c>
+      <c r="B1065">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1066">
+        <v>10</v>
+      </c>
+      <c r="B1066">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1067">
+        <v>1</v>
+      </c>
+      <c r="B1067">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1068">
+        <v>16</v>
+      </c>
+      <c r="B1068">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1069">
+        <v>16</v>
+      </c>
+      <c r="B1069">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1070">
+        <v>7</v>
+      </c>
+      <c r="B1070">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1071">
+        <v>5</v>
+      </c>
+      <c r="B1071">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1072">
+        <v>3</v>
+      </c>
+      <c r="B1072">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1073">
+        <v>6</v>
+      </c>
+      <c r="B1073">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1074">
+        <v>9</v>
+      </c>
+      <c r="B1074">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1075">
+        <v>4</v>
+      </c>
+      <c r="B1075">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1076">
+        <v>7</v>
+      </c>
+      <c r="B1076">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1077">
+        <v>7</v>
+      </c>
+      <c r="B1077">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1078">
+        <v>4</v>
+      </c>
+      <c r="B1078">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1079">
+        <v>1</v>
+      </c>
+      <c r="B1079">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1080">
+        <v>10</v>
+      </c>
+      <c r="B1080">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1081">
+        <v>11</v>
+      </c>
+      <c r="B1081">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1082">
+        <v>18</v>
+      </c>
+      <c r="B1082">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1083">
+        <v>7</v>
+      </c>
+      <c r="B1083">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1084">
+        <v>19</v>
+      </c>
+      <c r="B1084">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1085">
+        <v>18</v>
+      </c>
+      <c r="B1085">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1086">
+        <v>17</v>
+      </c>
+      <c r="B1086">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1087">
+        <v>4</v>
+      </c>
+      <c r="B1087">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1088">
+        <v>9</v>
+      </c>
+      <c r="B1088">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1089">
+        <v>19</v>
+      </c>
+      <c r="B1089">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1090">
+        <v>7</v>
+      </c>
+      <c r="B1090">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1091">
+        <v>20</v>
+      </c>
+      <c r="B1091">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1092">
+        <v>18</v>
+      </c>
+      <c r="B1092">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1093">
+        <v>5</v>
+      </c>
+      <c r="B1093">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1094">
+        <v>7</v>
+      </c>
+      <c r="B1094">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1095">
+        <v>2</v>
+      </c>
+      <c r="B1095">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1096">
+        <v>3</v>
+      </c>
+      <c r="B1096">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1097">
+        <v>4</v>
+      </c>
+      <c r="B1097">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1098">
+        <v>7</v>
+      </c>
+      <c r="B1098">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1099">
+        <v>16</v>
+      </c>
+      <c r="B1099">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1100">
+        <v>11</v>
+      </c>
+      <c r="B1100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1101">
+        <v>4</v>
+      </c>
+      <c r="B1101">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1102">
+        <v>6</v>
+      </c>
+      <c r="B1102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1103">
+        <v>13</v>
+      </c>
+      <c r="B1103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1104">
+        <v>12</v>
+      </c>
+      <c r="B1104">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1105">
+        <v>1</v>
+      </c>
+      <c r="B1105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1106">
+        <v>7</v>
+      </c>
+      <c r="B1106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1107">
+        <v>11</v>
+      </c>
+      <c r="B1107">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1108">
+        <v>6</v>
+      </c>
+      <c r="B1108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1109">
+        <v>1</v>
+      </c>
+      <c r="B1109">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1110">
+        <v>1</v>
+      </c>
+      <c r="B1110">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1111">
+        <v>18</v>
+      </c>
+      <c r="B1111">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1112">
+        <v>2</v>
+      </c>
+      <c r="B1112">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1113">
+        <v>7</v>
+      </c>
+      <c r="B1113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1114">
+        <v>16</v>
+      </c>
+      <c r="B1114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1115">
+        <v>13</v>
+      </c>
+      <c r="B1115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1116">
+        <v>14</v>
+      </c>
+      <c r="B1116">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1117">
+        <v>7</v>
+      </c>
+      <c r="B1117">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1118">
+        <v>19</v>
+      </c>
+      <c r="B1118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1119">
+        <v>9</v>
+      </c>
+      <c r="B1119">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1120">
+        <v>16</v>
+      </c>
+      <c r="B1120">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1121">
+        <v>6</v>
+      </c>
+      <c r="B1121">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1122">
+        <v>9</v>
+      </c>
+      <c r="B1122">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1123">
+        <v>9</v>
+      </c>
+      <c r="B1123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1124">
+        <v>10</v>
+      </c>
+      <c r="B1124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1125">
+        <v>19</v>
+      </c>
+      <c r="B1125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1126">
+        <v>3</v>
+      </c>
+      <c r="B1126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1127">
+        <v>13</v>
+      </c>
+      <c r="B1127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1128">
+        <v>8</v>
+      </c>
+      <c r="B1128">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1129">
+        <v>14</v>
+      </c>
+      <c r="B1129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1130">
+        <v>18</v>
+      </c>
+      <c r="B1130">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1131">
+        <v>5</v>
+      </c>
+      <c r="B1131">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1132">
+        <v>7</v>
+      </c>
+      <c r="B1132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1133">
+        <v>20</v>
+      </c>
+      <c r="B1133">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1134">
+        <v>5</v>
+      </c>
+      <c r="B1134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1135">
+        <v>16</v>
+      </c>
+      <c r="B1135">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1136">
+        <v>14</v>
+      </c>
+      <c r="B1136">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1137">
+        <v>19</v>
+      </c>
+      <c r="B1137">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1138">
+        <v>3</v>
+      </c>
+      <c r="B1138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1139">
+        <v>3</v>
+      </c>
+      <c r="B1139">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1140">
+        <v>8</v>
+      </c>
+      <c r="B1140">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1141">
+        <v>9</v>
+      </c>
+      <c r="B1141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1142">
+        <v>18</v>
+      </c>
+      <c r="B1142">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1143">
+        <v>5</v>
+      </c>
+      <c r="B1143">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1144">
+        <v>9</v>
+      </c>
+      <c r="B1144">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1145">
+        <v>15</v>
+      </c>
+      <c r="B1145">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1146">
+        <v>4</v>
+      </c>
+      <c r="B1146">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1147">
+        <v>18</v>
+      </c>
+      <c r="B1147">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1148">
+        <v>12</v>
+      </c>
+      <c r="B1148">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1149">
+        <v>11</v>
+      </c>
+      <c r="B1149">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1150">
+        <v>5</v>
+      </c>
+      <c r="B1150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1151">
+        <v>10</v>
+      </c>
+      <c r="B1151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1152">
+        <v>5</v>
+      </c>
+      <c r="B1152">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1153">
+        <v>1</v>
+      </c>
+      <c r="B1153">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1154">
+        <v>3</v>
+      </c>
+      <c r="B1154">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1155">
+        <v>12</v>
+      </c>
+      <c r="B1155">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1156">
+        <v>4</v>
+      </c>
+      <c r="B1156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1157">
+        <v>7</v>
+      </c>
+      <c r="B1157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1158">
+        <v>13</v>
+      </c>
+      <c r="B1158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1159">
+        <v>7</v>
+      </c>
+      <c r="B1159">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1160">
+        <v>14</v>
+      </c>
+      <c r="B1160">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1161">
+        <v>19</v>
+      </c>
+      <c r="B1161">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1162">
+        <v>12</v>
+      </c>
+      <c r="B1162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1163">
+        <v>2</v>
+      </c>
+      <c r="B1163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1164">
+        <v>6</v>
+      </c>
+      <c r="B1164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1165">
+        <v>14</v>
+      </c>
+      <c r="B1165">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1166">
+        <v>3</v>
+      </c>
+      <c r="B1166">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1167">
+        <v>9</v>
+      </c>
+      <c r="B1167">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1168">
+        <v>20</v>
+      </c>
+      <c r="B1168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1169">
+        <v>7</v>
+      </c>
+      <c r="B1169">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1170">
+        <v>19</v>
+      </c>
+      <c r="B1170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1171">
+        <v>13</v>
+      </c>
+      <c r="B1171">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1172">
+        <v>10</v>
+      </c>
+      <c r="B1172">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1173">
+        <v>4</v>
+      </c>
+      <c r="B1173">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1174">
+        <v>12</v>
+      </c>
+      <c r="B1174">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1175">
+        <v>12</v>
+      </c>
+      <c r="B1175">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1176">
+        <v>8</v>
+      </c>
+      <c r="B1176">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1177">
+        <v>19</v>
+      </c>
+      <c r="B1177">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1178">
+        <v>5</v>
+      </c>
+      <c r="B1178">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1179">
+        <v>3</v>
+      </c>
+      <c r="B1179">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1180">
+        <v>2</v>
+      </c>
+      <c r="B1180">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1181">
+        <v>18</v>
+      </c>
+      <c r="B1181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1182">
+        <v>5</v>
+      </c>
+      <c r="B1182">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1183">
+        <v>16</v>
+      </c>
+      <c r="B1183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1184">
+        <v>20</v>
+      </c>
+      <c r="B1184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1185">
+        <v>5</v>
+      </c>
+      <c r="B1185">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1186">
+        <v>14</v>
+      </c>
+      <c r="B1186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1187">
+        <v>7</v>
+      </c>
+      <c r="B1187">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1188">
+        <v>19</v>
+      </c>
+      <c r="B1188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1189">
+        <v>3</v>
+      </c>
+      <c r="B1189">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1190">
+        <v>20</v>
+      </c>
+      <c r="B1190">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1191">
+        <v>18</v>
+      </c>
+      <c r="B1191">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1192">
+        <v>9</v>
+      </c>
+      <c r="B1192">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1193">
+        <v>19</v>
+      </c>
+      <c r="B1193">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1194">
+        <v>16</v>
+      </c>
+      <c r="B1194">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1195">
+        <v>2</v>
+      </c>
+      <c r="B1195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1196">
+        <v>7</v>
+      </c>
+      <c r="B1196">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1197">
+        <v>11</v>
+      </c>
+      <c r="B1197">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1198">
+        <v>19</v>
+      </c>
+      <c r="B1198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1199">
+        <v>8</v>
+      </c>
+      <c r="B1199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1200">
+        <v>2</v>
+      </c>
+      <c r="B1200">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1201">
+        <v>2</v>
+      </c>
+      <c r="B1201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1202">
+        <v>12</v>
+      </c>
+      <c r="B1202">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1203">
+        <v>11</v>
+      </c>
+      <c r="B1203">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1204">
+        <v>19</v>
+      </c>
+      <c r="B1204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1205">
+        <v>6</v>
+      </c>
+      <c r="B1205">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1206">
+        <v>17</v>
+      </c>
+      <c r="B1206">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1207">
+        <v>11</v>
+      </c>
+      <c r="B1207">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1208">
+        <v>18</v>
+      </c>
+      <c r="B1208">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1209">
+        <v>3</v>
+      </c>
+      <c r="B1209">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1210">
+        <v>4</v>
+      </c>
+      <c r="B1210">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1211">
+        <v>15</v>
+      </c>
+      <c r="B1211">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1212">
+        <v>20</v>
+      </c>
+      <c r="B1212">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1213">
+        <v>20</v>
+      </c>
+      <c r="B1213">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1214">
+        <v>1</v>
+      </c>
+      <c r="B1214">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1215">
+        <v>10</v>
+      </c>
+      <c r="B1215">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1216">
+        <v>5</v>
+      </c>
+      <c r="B1216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1217">
+        <v>12</v>
+      </c>
+      <c r="B1217">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1218">
+        <v>5</v>
+      </c>
+      <c r="B1218">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1219">
+        <v>11</v>
+      </c>
+      <c r="B1219">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1220">
+        <v>15</v>
+      </c>
+      <c r="B1220">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1221">
+        <v>11</v>
+      </c>
+      <c r="B1221">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1222">
+        <v>11</v>
+      </c>
+      <c r="B1222">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1223">
+        <v>9</v>
+      </c>
+      <c r="B1223">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1224">
+        <v>17</v>
+      </c>
+      <c r="B1224">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1225">
+        <v>11</v>
+      </c>
+      <c r="B1225">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1226">
+        <v>5</v>
+      </c>
+      <c r="B1226">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1227">
+        <v>12</v>
+      </c>
+      <c r="B1227">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1228">
+        <v>9</v>
+      </c>
+      <c r="B1228">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1229">
+        <v>8</v>
+      </c>
+      <c r="B1229">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1230">
+        <v>4</v>
+      </c>
+      <c r="B1230">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1231">
+        <v>19</v>
+      </c>
+      <c r="B1231">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1232">
+        <v>17</v>
+      </c>
+      <c r="B1232">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1233">
+        <v>15</v>
+      </c>
+      <c r="B1233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1234">
+        <v>4</v>
+      </c>
+      <c r="B1234">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1235">
+        <v>5</v>
+      </c>
+      <c r="B1235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1236">
+        <v>16</v>
+      </c>
+      <c r="B1236">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1237">
+        <v>10</v>
+      </c>
+      <c r="B1237">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1238">
+        <v>7</v>
+      </c>
+      <c r="B1238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1239">
+        <v>2</v>
+      </c>
+      <c r="B1239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1240">
+        <v>9</v>
+      </c>
+      <c r="B1240">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1241">
+        <v>9</v>
+      </c>
+      <c r="B1241">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1242">
+        <v>9</v>
+      </c>
+      <c r="B1242">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1243">
+        <v>7</v>
+      </c>
+      <c r="B1243">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1244">
+        <v>8</v>
+      </c>
+      <c r="B1244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1245">
+        <v>8</v>
+      </c>
+      <c r="B1245">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1246">
+        <v>2</v>
+      </c>
+      <c r="B1246">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1247">
+        <v>6</v>
+      </c>
+      <c r="B1247">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1248">
+        <v>2</v>
+      </c>
+      <c r="B1248">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1249">
+        <v>1</v>
+      </c>
+      <c r="B1249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1250">
+        <v>12</v>
+      </c>
+      <c r="B1250">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1251">
+        <v>19</v>
+      </c>
+      <c r="B1251">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1252">
+        <v>10</v>
+      </c>
+      <c r="B1252">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1253">
+        <v>11</v>
+      </c>
+      <c r="B1253">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1254">
+        <v>3</v>
+      </c>
+      <c r="B1254">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1255">
+        <v>14</v>
+      </c>
+      <c r="B1255">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1256">
+        <v>18</v>
+      </c>
+      <c r="B1256">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1257">
+        <v>2</v>
+      </c>
+      <c r="B1257">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1258">
+        <v>19</v>
+      </c>
+      <c r="B1258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1259">
+        <v>11</v>
+      </c>
+      <c r="B1259">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1260">
+        <v>6</v>
+      </c>
+      <c r="B1260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1261">
+        <v>13</v>
+      </c>
+      <c r="B1261">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1262">
+        <v>1</v>
+      </c>
+      <c r="B1262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1263">
+        <v>9</v>
+      </c>
+      <c r="B1263">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1264">
+        <v>1</v>
+      </c>
+      <c r="B1264">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1265">
+        <v>3</v>
+      </c>
+      <c r="B1265">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1266">
+        <v>10</v>
+      </c>
+      <c r="B1266">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1267">
+        <v>7</v>
+      </c>
+      <c r="B1267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1268">
+        <v>20</v>
+      </c>
+      <c r="B1268">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1269">
+        <v>16</v>
+      </c>
+      <c r="B1269">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1270">
+        <v>16</v>
+      </c>
+      <c r="B1270">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1271">
+        <v>17</v>
+      </c>
+      <c r="B1271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1272">
+        <v>3</v>
+      </c>
+      <c r="B1272">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1273">
+        <v>20</v>
+      </c>
+      <c r="B1273">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1274">
+        <v>2</v>
+      </c>
+      <c r="B1274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1275">
+        <v>17</v>
+      </c>
+      <c r="B1275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1276">
+        <v>18</v>
+      </c>
+      <c r="B1276">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1277">
+        <v>15</v>
+      </c>
+      <c r="B1277">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1278">
+        <v>17</v>
+      </c>
+      <c r="B1278">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1279">
+        <v>10</v>
+      </c>
+      <c r="B1279">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1280">
+        <v>20</v>
+      </c>
+      <c r="B1280">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1281">
+        <v>12</v>
+      </c>
+      <c r="B1281">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1282">
+        <v>13</v>
+      </c>
+      <c r="B1282">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1283">
+        <v>4</v>
+      </c>
+      <c r="B1283">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1284">
+        <v>20</v>
+      </c>
+      <c r="B1284">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1285">
+        <v>15</v>
+      </c>
+      <c r="B1285">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1286">
+        <v>10</v>
+      </c>
+      <c r="B1286">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1287">
+        <v>12</v>
+      </c>
+      <c r="B1287">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1288">
+        <v>20</v>
+      </c>
+      <c r="B1288">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1289">
+        <v>11</v>
+      </c>
+      <c r="B1289">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1290">
+        <v>15</v>
+      </c>
+      <c r="B1290">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1291">
+        <v>1</v>
+      </c>
+      <c r="B1291">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1292">
+        <v>18</v>
+      </c>
+      <c r="B1292">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1293">
+        <v>17</v>
+      </c>
+      <c r="B1293">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1294">
+        <v>6</v>
+      </c>
+      <c r="B1294">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1295">
+        <v>5</v>
+      </c>
+      <c r="B1295">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1296">
+        <v>1</v>
+      </c>
+      <c r="B1296">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1297">
+        <v>19</v>
+      </c>
+      <c r="B1297">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1298">
+        <v>9</v>
+      </c>
+      <c r="B1298">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1299">
+        <v>6</v>
+      </c>
+      <c r="B1299">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1300">
+        <v>12</v>
+      </c>
+      <c r="B1300">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1301">
+        <v>17</v>
+      </c>
+      <c r="B1301">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1302">
+        <v>17</v>
+      </c>
+      <c r="B1302">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1303">
+        <v>14</v>
+      </c>
+      <c r="B1303">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1304">
+        <v>19</v>
+      </c>
+      <c r="B1304">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1305">
+        <v>8</v>
+      </c>
+      <c r="B1305">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1306">
+        <v>4</v>
+      </c>
+      <c r="B1306">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1307">
+        <v>13</v>
+      </c>
+      <c r="B1307">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1308">
+        <v>20</v>
+      </c>
+      <c r="B1308">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1309">
+        <v>13</v>
+      </c>
+      <c r="B1309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1310">
+        <v>11</v>
+      </c>
+      <c r="B1310">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1311">
+        <v>16</v>
+      </c>
+      <c r="B1311">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1312">
+        <v>13</v>
+      </c>
+      <c r="B1312">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1313">
+        <v>3</v>
+      </c>
+      <c r="B1313">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1314">
+        <v>7</v>
+      </c>
+      <c r="B1314">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1315">
+        <v>11</v>
+      </c>
+      <c r="B1315">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1316">
+        <v>19</v>
+      </c>
+      <c r="B1316">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1317">
+        <v>19</v>
+      </c>
+      <c r="B1317">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1318">
+        <v>8</v>
+      </c>
+      <c r="B1318">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1319">
+        <v>1</v>
+      </c>
+      <c r="B1319">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1320">
+        <v>3</v>
+      </c>
+      <c r="B1320">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1321">
+        <v>12</v>
+      </c>
+      <c r="B1321">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1322">
+        <v>2</v>
+      </c>
+      <c r="B1322">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1323">
+        <v>10</v>
+      </c>
+      <c r="B1323">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1324">
+        <v>19</v>
+      </c>
+      <c r="B1324">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1325">
+        <v>19</v>
+      </c>
+      <c r="B1325">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1326">
+        <v>2</v>
+      </c>
+      <c r="B1326">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1327">
+        <v>12</v>
+      </c>
+      <c r="B1327">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1328">
+        <v>18</v>
+      </c>
+      <c r="B1328">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1329">
+        <v>6</v>
+      </c>
+      <c r="B1329">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1330">
+        <v>11</v>
+      </c>
+      <c r="B1330">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1331">
+        <v>11</v>
+      </c>
+      <c r="B1331">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1332">
+        <v>12</v>
+      </c>
+      <c r="B1332">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1333">
+        <v>14</v>
+      </c>
+      <c r="B1333">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1334">
+        <v>18</v>
+      </c>
+      <c r="B1334">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1335">
+        <v>13</v>
+      </c>
+      <c r="B1335">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1336">
+        <v>14</v>
+      </c>
+      <c r="B1336">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1337">
+        <v>1</v>
+      </c>
+      <c r="B1337">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1338">
+        <v>8</v>
+      </c>
+      <c r="B1338">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1339">
+        <v>19</v>
+      </c>
+      <c r="B1339">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1340">
+        <v>12</v>
+      </c>
+      <c r="B1340">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1341">
+        <v>11</v>
+      </c>
+      <c r="B1341">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1342">
+        <v>2</v>
+      </c>
+      <c r="B1342">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1343">
+        <v>14</v>
+      </c>
+      <c r="B1343">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1344">
+        <v>3</v>
+      </c>
+      <c r="B1344">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1345">
+        <v>18</v>
+      </c>
+      <c r="B1345">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1346">
+        <v>9</v>
+      </c>
+      <c r="B1346">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1347">
+        <v>9</v>
+      </c>
+      <c r="B1347">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1348">
+        <v>8</v>
+      </c>
+      <c r="B1348">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1349">
+        <v>3</v>
+      </c>
+      <c r="B1349">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1350">
+        <v>2</v>
+      </c>
+      <c r="B1350">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1351">
+        <v>12</v>
+      </c>
+      <c r="B1351">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1352">
+        <v>13</v>
+      </c>
+      <c r="B1352">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1353">
+        <v>1</v>
+      </c>
+      <c r="B1353">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1354">
+        <v>13</v>
+      </c>
+      <c r="B1354">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1355">
+        <v>18</v>
+      </c>
+      <c r="B1355">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1356">
+        <v>11</v>
+      </c>
+      <c r="B1356">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1357">
+        <v>2</v>
+      </c>
+      <c r="B1357">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1358">
+        <v>1</v>
+      </c>
+      <c r="B1358">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1359">
+        <v>4</v>
+      </c>
+      <c r="B1359">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1360">
+        <v>9</v>
+      </c>
+      <c r="B1360">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1361">
+        <v>11</v>
+      </c>
+      <c r="B1361">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1362">
+        <v>18</v>
+      </c>
+      <c r="B1362">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1363">
+        <v>19</v>
+      </c>
+      <c r="B1363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1364">
+        <v>12</v>
+      </c>
+      <c r="B1364">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1365">
+        <v>3</v>
+      </c>
+      <c r="B1365">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1366">
+        <v>20</v>
+      </c>
+      <c r="B1366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1367">
+        <v>20</v>
+      </c>
+      <c r="B1367">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1368">
+        <v>1</v>
+      </c>
+      <c r="B1368">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1369">
+        <v>3</v>
+      </c>
+      <c r="B1369">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1370">
+        <v>11</v>
+      </c>
+      <c r="B1370">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1371">
+        <v>10</v>
+      </c>
+      <c r="B1371">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1372">
+        <v>6</v>
+      </c>
+      <c r="B1372">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1373">
+        <v>15</v>
+      </c>
+      <c r="B1373">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1374">
+        <v>9</v>
+      </c>
+      <c r="B1374">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1375">
+        <v>16</v>
+      </c>
+      <c r="B1375">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1376">
+        <v>2</v>
+      </c>
+      <c r="B1376">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1377">
+        <v>14</v>
+      </c>
+      <c r="B1377">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1378">
+        <v>7</v>
+      </c>
+      <c r="B1378">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1379">
+        <v>2</v>
+      </c>
+      <c r="B1379">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1380">
+        <v>9</v>
+      </c>
+      <c r="B1380">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1381">
+        <v>18</v>
+      </c>
+      <c r="B1381">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1382">
+        <v>14</v>
+      </c>
+      <c r="B1382">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1383">
+        <v>19</v>
+      </c>
+      <c r="B1383">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1384">
+        <v>12</v>
+      </c>
+      <c r="B1384">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1385">
+        <v>1</v>
+      </c>
+      <c r="B1385">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1386">
+        <v>17</v>
+      </c>
+      <c r="B1386">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1387">
+        <v>7</v>
+      </c>
+      <c r="B1387">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1388">
+        <v>12</v>
+      </c>
+      <c r="B1388">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1389">
+        <v>6</v>
+      </c>
+      <c r="B1389">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1390">
+        <v>12</v>
+      </c>
+      <c r="B1390">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1391">
+        <v>17</v>
+      </c>
+      <c r="B1391">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1392">
+        <v>14</v>
+      </c>
+      <c r="B1392">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1393">
+        <v>16</v>
+      </c>
+      <c r="B1393">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1394">
+        <v>19</v>
+      </c>
+      <c r="B1394">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1395">
+        <v>1</v>
+      </c>
+      <c r="B1395">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1396">
+        <v>7</v>
+      </c>
+      <c r="B1396">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1397">
+        <v>6</v>
+      </c>
+      <c r="B1397">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1398">
+        <v>2</v>
+      </c>
+      <c r="B1398">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1399">
+        <v>1</v>
+      </c>
+      <c r="B1399">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1400">
+        <v>15</v>
+      </c>
+      <c r="B1400">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1401">
+        <v>10</v>
+      </c>
+      <c r="B1401">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1402">
+        <v>1</v>
+      </c>
+      <c r="B1402">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1403">
+        <v>2</v>
+      </c>
+      <c r="B1403">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1404">
+        <v>13</v>
+      </c>
+      <c r="B1404">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1405">
+        <v>18</v>
+      </c>
+      <c r="B1405">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1406">
+        <v>20</v>
+      </c>
+      <c r="B1406">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1407">
+        <v>8</v>
+      </c>
+      <c r="B1407">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1408">
+        <v>16</v>
+      </c>
+      <c r="B1408">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1409">
+        <v>19</v>
+      </c>
+      <c r="B1409">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1410">
+        <v>9</v>
+      </c>
+      <c r="B1410">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1411">
+        <v>13</v>
+      </c>
+      <c r="B1411">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1412">
+        <v>7</v>
+      </c>
+      <c r="B1412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1413">
+        <v>19</v>
+      </c>
+      <c r="B1413">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1414">
+        <v>15</v>
+      </c>
+      <c r="B1414">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1415">
+        <v>7</v>
+      </c>
+      <c r="B1415">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1416">
+        <v>8</v>
+      </c>
+      <c r="B1416">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1417">
+        <v>15</v>
+      </c>
+      <c r="B1417">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1418">
+        <v>13</v>
+      </c>
+      <c r="B1418">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1419">
+        <v>15</v>
+      </c>
+      <c r="B1419">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1420">
+        <v>12</v>
+      </c>
+      <c r="B1420">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1421">
+        <v>13</v>
+      </c>
+      <c r="B1421">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1422">
+        <v>20</v>
+      </c>
+      <c r="B1422">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1423">
+        <v>19</v>
+      </c>
+      <c r="B1423">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1424">
+        <v>5</v>
+      </c>
+      <c r="B1424">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1425">
+        <v>12</v>
+      </c>
+      <c r="B1425">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1426">
+        <v>19</v>
+      </c>
+      <c r="B1426">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1427">
+        <v>20</v>
+      </c>
+      <c r="B1427">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1428">
+        <v>4</v>
+      </c>
+      <c r="B1428">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1429">
+        <v>12</v>
+      </c>
+      <c r="B1429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1430">
+        <v>17</v>
+      </c>
+      <c r="B1430">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1431">
+        <v>12</v>
+      </c>
+      <c r="B1431">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1432">
+        <v>2</v>
+      </c>
+      <c r="B1432">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1433">
+        <v>10</v>
+      </c>
+      <c r="B1433">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1434">
+        <v>2</v>
+      </c>
+      <c r="B1434">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1435">
+        <v>11</v>
+      </c>
+      <c r="B1435">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1436">
+        <v>20</v>
+      </c>
+      <c r="B1436">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1437">
+        <v>8</v>
+      </c>
+      <c r="B1437">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1438">
+        <v>4</v>
+      </c>
+      <c r="B1438">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1439">
+        <v>9</v>
+      </c>
+      <c r="B1439">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1440">
+        <v>20</v>
+      </c>
+      <c r="B1440">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1441">
+        <v>3</v>
+      </c>
+      <c r="B1441">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1442">
+        <v>11</v>
+      </c>
+      <c r="B1442">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1443">
+        <v>17</v>
+      </c>
+      <c r="B1443">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1444">
+        <v>17</v>
+      </c>
+      <c r="B1444">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1445">
+        <v>2</v>
+      </c>
+      <c r="B1445">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1446">
+        <v>15</v>
+      </c>
+      <c r="B1446">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1447">
+        <v>14</v>
+      </c>
+      <c r="B1447">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1448">
+        <v>11</v>
+      </c>
+      <c r="B1448">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1449">
+        <v>3</v>
+      </c>
+      <c r="B1449">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1450">
+        <v>19</v>
+      </c>
+      <c r="B1450">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1451">
+        <v>7</v>
+      </c>
+      <c r="B1451">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1452">
+        <v>19</v>
+      </c>
+      <c r="B1452">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1453">
+        <v>12</v>
+      </c>
+      <c r="B1453">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1454">
+        <v>19</v>
+      </c>
+      <c r="B1454">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1455">
+        <v>11</v>
+      </c>
+      <c r="B1455">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1456">
+        <v>13</v>
+      </c>
+      <c r="B1456">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1457">
+        <v>19</v>
+      </c>
+      <c r="B1457">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1458">
+        <v>17</v>
+      </c>
+      <c r="B1458">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1459">
+        <v>20</v>
+      </c>
+      <c r="B1459">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1460">
+        <v>6</v>
+      </c>
+      <c r="B1460">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1461">
+        <v>11</v>
+      </c>
+      <c r="B1461">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1462">
+        <v>11</v>
+      </c>
+      <c r="B1462">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1463">
+        <v>16</v>
+      </c>
+      <c r="B1463">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1464">
+        <v>17</v>
+      </c>
+      <c r="B1464">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1465">
+        <v>17</v>
+      </c>
+      <c r="B1465">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1466">
+        <v>12</v>
+      </c>
+      <c r="B1466">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1467">
+        <v>20</v>
+      </c>
+      <c r="B1467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1468">
+        <v>7</v>
+      </c>
+      <c r="B1468">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1469">
+        <v>4</v>
+      </c>
+      <c r="B1469">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1470">
+        <v>9</v>
+      </c>
+      <c r="B1470">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1471">
+        <v>2</v>
+      </c>
+      <c r="B1471">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1472">
+        <v>4</v>
+      </c>
+      <c r="B1472">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1473">
+        <v>19</v>
+      </c>
+      <c r="B1473">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1474">
+        <v>18</v>
+      </c>
+      <c r="B1474">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1475">
+        <v>3</v>
+      </c>
+      <c r="B1475">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1476">
+        <v>13</v>
+      </c>
+      <c r="B1476">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1477">
+        <v>12</v>
+      </c>
+      <c r="B1477">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1478">
+        <v>5</v>
+      </c>
+      <c r="B1478">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1479">
+        <v>20</v>
+      </c>
+      <c r="B1479">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1480">
+        <v>10</v>
+      </c>
+      <c r="B1480">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1481">
+        <v>17</v>
+      </c>
+      <c r="B1481">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1482">
+        <v>4</v>
+      </c>
+      <c r="B1482">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1483">
+        <v>15</v>
+      </c>
+      <c r="B1483">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1484">
+        <v>14</v>
+      </c>
+      <c r="B1484">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1485">
+        <v>12</v>
+      </c>
+      <c r="B1485">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1486">
+        <v>12</v>
+      </c>
+      <c r="B1486">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1487">
+        <v>14</v>
+      </c>
+      <c r="B1487">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1488">
+        <v>7</v>
+      </c>
+      <c r="B1488">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1489">
+        <v>14</v>
+      </c>
+      <c r="B1489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1490">
+        <v>16</v>
+      </c>
+      <c r="B1490">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1491">
+        <v>11</v>
+      </c>
+      <c r="B1491">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1492">
+        <v>3</v>
+      </c>
+      <c r="B1492">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1493">
+        <v>20</v>
+      </c>
+      <c r="B1493">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1494">
+        <v>1</v>
+      </c>
+      <c r="B1494">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1495">
+        <v>20</v>
+      </c>
+      <c r="B1495">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1496">
+        <v>3</v>
+      </c>
+      <c r="B1496">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1497">
+        <v>14</v>
+      </c>
+      <c r="B1497">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1498">
+        <v>5</v>
+      </c>
+      <c r="B1498">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1499">
+        <v>8</v>
+      </c>
+      <c r="B1499">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1500">
+        <v>6</v>
+      </c>
+      <c r="B1500">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1501">
+        <v>19</v>
+      </c>
+      <c r="B1501">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1502">
+        <v>15</v>
+      </c>
+      <c r="B1502">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1503">
+        <v>9</v>
+      </c>
+      <c r="B1503">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1504">
+        <v>12</v>
+      </c>
+      <c r="B1504">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1505">
+        <v>3</v>
+      </c>
+      <c r="B1505">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1506">
+        <v>18</v>
+      </c>
+      <c r="B1506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1507">
+        <v>6</v>
+      </c>
+      <c r="B1507">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1508">
+        <v>4</v>
+      </c>
+      <c r="B1508">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1509">
+        <v>4</v>
+      </c>
+      <c r="B1509">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1510">
+        <v>5</v>
+      </c>
+      <c r="B1510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1511">
+        <v>1</v>
+      </c>
+      <c r="B1511">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1512">
+        <v>12</v>
+      </c>
+      <c r="B1512">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1513">
+        <v>2</v>
+      </c>
+      <c r="B1513">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1514">
+        <v>19</v>
+      </c>
+      <c r="B1514">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1515">
+        <v>20</v>
+      </c>
+      <c r="B1515">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1516">
+        <v>16</v>
+      </c>
+      <c r="B1516">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1517">
+        <v>9</v>
+      </c>
+      <c r="B1517">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1518">
+        <v>11</v>
+      </c>
+      <c r="B1518">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1519">
+        <v>14</v>
+      </c>
+      <c r="B1519">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1520">
+        <v>8</v>
+      </c>
+      <c r="B1520">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1521">
+        <v>18</v>
+      </c>
+      <c r="B1521">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1522">
+        <v>14</v>
+      </c>
+      <c r="B1522">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1523">
+        <v>15</v>
+      </c>
+      <c r="B1523">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1524">
+        <v>7</v>
+      </c>
+      <c r="B1524">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1525">
+        <v>18</v>
+      </c>
+      <c r="B1525">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1526">
+        <v>14</v>
+      </c>
+      <c r="B1526">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1527">
+        <v>19</v>
+      </c>
+      <c r="B1527">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1528">
+        <v>17</v>
+      </c>
+      <c r="B1528">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1529">
+        <v>5</v>
+      </c>
+      <c r="B1529">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1530">
+        <v>10</v>
+      </c>
+      <c r="B1530">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1531">
+        <v>14</v>
+      </c>
+      <c r="B1531">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1532">
+        <v>8</v>
+      </c>
+      <c r="B1532">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1533">
+        <v>6</v>
+      </c>
+      <c r="B1533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1534">
+        <v>16</v>
+      </c>
+      <c r="B1534">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1535">
+        <v>20</v>
+      </c>
+      <c r="B1535">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1536">
+        <v>17</v>
+      </c>
+      <c r="B1536">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1537">
+        <v>17</v>
+      </c>
+      <c r="B1537">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1538">
+        <v>6</v>
+      </c>
+      <c r="B1538">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1539">
+        <v>11</v>
+      </c>
+      <c r="B1539">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1540">
+        <v>11</v>
+      </c>
+      <c r="B1540">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1541">
+        <v>3</v>
+      </c>
+      <c r="B1541">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1542">
+        <v>20</v>
+      </c>
+      <c r="B1542">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1543">
+        <v>17</v>
+      </c>
+      <c r="B1543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1544">
+        <v>17</v>
+      </c>
+      <c r="B1544">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1545">
+        <v>7</v>
+      </c>
+      <c r="B1545">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1546">
+        <v>7</v>
+      </c>
+      <c r="B1546">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1547">
+        <v>11</v>
+      </c>
+      <c r="B1547">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1548">
+        <v>17</v>
+      </c>
+      <c r="B1548">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1549">
+        <v>9</v>
+      </c>
+      <c r="B1549">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1550">
+        <v>8</v>
+      </c>
+      <c r="B1550">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1551">
+        <v>12</v>
+      </c>
+      <c r="B1551">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1552">
+        <v>1</v>
+      </c>
+      <c r="B1552">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1553">
+        <v>9</v>
+      </c>
+      <c r="B1553">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1554">
+        <v>6</v>
+      </c>
+      <c r="B1554">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1555">
+        <v>8</v>
+      </c>
+      <c r="B1555">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1556">
+        <v>13</v>
+      </c>
+      <c r="B1556">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fresh rolls, minor display updates
</commit_message>
<xml_diff>
--- a/Dice_test.xlsx
+++ b/Dice_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmullens/Documents/GitHub/Dice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA89CDB-D259-344B-8518-C1DE1B3D61D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92AA9A8-89A6-044E-B9E5-4E4FAC447DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16160" xr2:uid="{D71FB28A-5275-6641-8EEB-6B08F00334B6}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Blue:</t>
   </si>
   <si>
-    <t>(Rolling on the flat wood desk, pick up and reroll after some shaking, avoid bumping into things near end of roll)</t>
+    <t>(Rolling on the flat wood desk, pick up and reroll after some shaking, avoid bumping into each other or objects near end of roll)</t>
   </si>
 </sst>
 </file>
@@ -394,11 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0194933F-D8D3-DD40-9924-A4C1D50508BE}">
-  <dimension ref="A1:F2302"/>
+  <dimension ref="A1:F2402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2303" sqref="A2303"/>
+      <pane ySplit="1" topLeftCell="A2370" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2403" sqref="A2403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18974,6 +18974,806 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2303">
+        <v>6</v>
+      </c>
+      <c r="B2303">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2304">
+        <v>2</v>
+      </c>
+      <c r="B2304">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2305">
+        <v>2</v>
+      </c>
+      <c r="B2305">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2306">
+        <v>3</v>
+      </c>
+      <c r="B2306">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2307">
+        <v>3</v>
+      </c>
+      <c r="B2307">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2308">
+        <v>18</v>
+      </c>
+      <c r="B2308">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2309">
+        <v>3</v>
+      </c>
+      <c r="B2309">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2310">
+        <v>12</v>
+      </c>
+      <c r="B2310">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2311">
+        <v>9</v>
+      </c>
+      <c r="B2311">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2312">
+        <v>2</v>
+      </c>
+      <c r="B2312">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2313">
+        <v>11</v>
+      </c>
+      <c r="B2313">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2314">
+        <v>9</v>
+      </c>
+      <c r="B2314">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2315">
+        <v>19</v>
+      </c>
+      <c r="B2315">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2316">
+        <v>4</v>
+      </c>
+      <c r="B2316">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2317">
+        <v>17</v>
+      </c>
+      <c r="B2317">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2318">
+        <v>6</v>
+      </c>
+      <c r="B2318">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2319">
+        <v>12</v>
+      </c>
+      <c r="B2319">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2320">
+        <v>8</v>
+      </c>
+      <c r="B2320">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2321">
+        <v>3</v>
+      </c>
+      <c r="B2321">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2322">
+        <v>1</v>
+      </c>
+      <c r="B2322">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2323">
+        <v>6</v>
+      </c>
+      <c r="B2323">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2324">
+        <v>3</v>
+      </c>
+      <c r="B2324">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2325">
+        <v>3</v>
+      </c>
+      <c r="B2325">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2326">
+        <v>17</v>
+      </c>
+      <c r="B2326">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2327">
+        <v>4</v>
+      </c>
+      <c r="B2327">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2328">
+        <v>10</v>
+      </c>
+      <c r="B2328">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2329">
+        <v>2</v>
+      </c>
+      <c r="B2329">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2330">
+        <v>10</v>
+      </c>
+      <c r="B2330">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2331">
+        <v>10</v>
+      </c>
+      <c r="B2331">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2332">
+        <v>18</v>
+      </c>
+      <c r="B2332">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2333">
+        <v>7</v>
+      </c>
+      <c r="B2333">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2334">
+        <v>9</v>
+      </c>
+      <c r="B2334">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2335">
+        <v>1</v>
+      </c>
+      <c r="B2335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2336">
+        <v>4</v>
+      </c>
+      <c r="B2336">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2337">
+        <v>18</v>
+      </c>
+      <c r="B2337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2338">
+        <v>3</v>
+      </c>
+      <c r="B2338">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2339">
+        <v>13</v>
+      </c>
+      <c r="B2339">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2340">
+        <v>12</v>
+      </c>
+      <c r="B2340">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2341">
+        <v>9</v>
+      </c>
+      <c r="B2341">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2342">
+        <v>13</v>
+      </c>
+      <c r="B2342">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2343">
+        <v>14</v>
+      </c>
+      <c r="B2343">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2344">
+        <v>17</v>
+      </c>
+      <c r="B2344">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2345">
+        <v>13</v>
+      </c>
+      <c r="B2345">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2346">
+        <v>11</v>
+      </c>
+      <c r="B2346">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2347">
+        <v>1</v>
+      </c>
+      <c r="B2347">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2348">
+        <v>19</v>
+      </c>
+      <c r="B2348">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2349">
+        <v>6</v>
+      </c>
+      <c r="B2349">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2350">
+        <v>3</v>
+      </c>
+      <c r="B2350">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2351">
+        <v>2</v>
+      </c>
+      <c r="B2351">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2352">
+        <v>18</v>
+      </c>
+      <c r="B2352">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2353">
+        <v>17</v>
+      </c>
+      <c r="B2353">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2354">
+        <v>17</v>
+      </c>
+      <c r="B2354">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2355">
+        <v>20</v>
+      </c>
+      <c r="B2355">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2356">
+        <v>9</v>
+      </c>
+      <c r="B2356">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2357">
+        <v>3</v>
+      </c>
+      <c r="B2357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2358">
+        <v>13</v>
+      </c>
+      <c r="B2358">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2359">
+        <v>18</v>
+      </c>
+      <c r="B2359">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2360">
+        <v>10</v>
+      </c>
+      <c r="B2360">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2361">
+        <v>13</v>
+      </c>
+      <c r="B2361">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2362">
+        <v>7</v>
+      </c>
+      <c r="B2362">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2363">
+        <v>16</v>
+      </c>
+      <c r="B2363">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2364">
+        <v>6</v>
+      </c>
+      <c r="B2364">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2365">
+        <v>12</v>
+      </c>
+      <c r="B2365">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2366">
+        <v>12</v>
+      </c>
+      <c r="B2366">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2367">
+        <v>11</v>
+      </c>
+      <c r="B2367">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2368">
+        <v>10</v>
+      </c>
+      <c r="B2368">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2369">
+        <v>2</v>
+      </c>
+      <c r="B2369">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2370">
+        <v>4</v>
+      </c>
+      <c r="B2370">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2371">
+        <v>6</v>
+      </c>
+      <c r="B2371">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2372">
+        <v>20</v>
+      </c>
+      <c r="B2372">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2373">
+        <v>18</v>
+      </c>
+      <c r="B2373">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2374">
+        <v>13</v>
+      </c>
+      <c r="B2374">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2375">
+        <v>3</v>
+      </c>
+      <c r="B2375">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2376">
+        <v>12</v>
+      </c>
+      <c r="B2376">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2377">
+        <v>12</v>
+      </c>
+      <c r="B2377">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2378">
+        <v>15</v>
+      </c>
+      <c r="B2378">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2379">
+        <v>13</v>
+      </c>
+      <c r="B2379">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2380">
+        <v>7</v>
+      </c>
+      <c r="B2380">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2381">
+        <v>9</v>
+      </c>
+      <c r="B2381">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2382">
+        <v>1</v>
+      </c>
+      <c r="B2382">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2383">
+        <v>4</v>
+      </c>
+      <c r="B2383">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2384">
+        <v>9</v>
+      </c>
+      <c r="B2384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2385">
+        <v>15</v>
+      </c>
+      <c r="B2385">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2386">
+        <v>19</v>
+      </c>
+      <c r="B2386">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2387">
+        <v>2</v>
+      </c>
+      <c r="B2387">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2388">
+        <v>10</v>
+      </c>
+      <c r="B2388">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2389">
+        <v>3</v>
+      </c>
+      <c r="B2389">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2390">
+        <v>11</v>
+      </c>
+      <c r="B2390">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2391">
+        <v>4</v>
+      </c>
+      <c r="B2391">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2392">
+        <v>3</v>
+      </c>
+      <c r="B2392">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2393">
+        <v>11</v>
+      </c>
+      <c r="B2393">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2394">
+        <v>15</v>
+      </c>
+      <c r="B2394">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2395">
+        <v>10</v>
+      </c>
+      <c r="B2395">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2396">
+        <v>11</v>
+      </c>
+      <c r="B2396">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2397">
+        <v>16</v>
+      </c>
+      <c r="B2397">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2398">
+        <v>15</v>
+      </c>
+      <c r="B2398">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2399">
+        <v>18</v>
+      </c>
+      <c r="B2399">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2400">
+        <v>14</v>
+      </c>
+      <c r="B2400">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2401">
+        <v>14</v>
+      </c>
+      <c r="B2401">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2402">
+        <v>2</v>
+      </c>
+      <c r="B2402">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Continuing updates to visualization and data collection
</commit_message>
<xml_diff>
--- a/Dice_test.xlsx
+++ b/Dice_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmullens/Documents/GitHub/Dice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92AA9A8-89A6-044E-B9E5-4E4FAC447DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9F9231-3002-0A45-95B4-66FFA2A2DF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16160" xr2:uid="{D71FB28A-5275-6641-8EEB-6B08F00334B6}"/>
   </bookViews>
@@ -394,11 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0194933F-D8D3-DD40-9924-A4C1D50508BE}">
-  <dimension ref="A1:F2402"/>
+  <dimension ref="A1:F2704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2370" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2403" sqref="A2403"/>
+      <pane ySplit="1" topLeftCell="A2672" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2705" sqref="A2705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19774,6 +19774,2422 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2403" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2403">
+        <v>10</v>
+      </c>
+      <c r="B2403">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2404">
+        <v>14</v>
+      </c>
+      <c r="B2404">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2405">
+        <v>7</v>
+      </c>
+      <c r="B2405">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2406">
+        <v>1</v>
+      </c>
+      <c r="B2406">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2407">
+        <v>7</v>
+      </c>
+      <c r="B2407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2408">
+        <v>12</v>
+      </c>
+      <c r="B2408">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2409">
+        <v>11</v>
+      </c>
+      <c r="B2409">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2410">
+        <v>10</v>
+      </c>
+      <c r="B2410">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2411">
+        <v>18</v>
+      </c>
+      <c r="B2411">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2412">
+        <v>4</v>
+      </c>
+      <c r="B2412">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2413">
+        <v>19</v>
+      </c>
+      <c r="B2413">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2414">
+        <v>4</v>
+      </c>
+      <c r="B2414">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2415">
+        <v>15</v>
+      </c>
+      <c r="B2415">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2416">
+        <v>5</v>
+      </c>
+      <c r="B2416">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2417">
+        <v>1</v>
+      </c>
+      <c r="B2417">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2418">
+        <v>17</v>
+      </c>
+      <c r="B2418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2419">
+        <v>6</v>
+      </c>
+      <c r="B2419">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2420">
+        <v>17</v>
+      </c>
+      <c r="B2420">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2421">
+        <v>2</v>
+      </c>
+      <c r="B2421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2422">
+        <v>7</v>
+      </c>
+      <c r="B2422">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2423">
+        <v>8</v>
+      </c>
+      <c r="B2423">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2424">
+        <v>19</v>
+      </c>
+      <c r="B2424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2425">
+        <v>3</v>
+      </c>
+      <c r="B2425">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2426">
+        <v>12</v>
+      </c>
+      <c r="B2426">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2427">
+        <v>1</v>
+      </c>
+      <c r="B2427">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2428">
+        <v>3</v>
+      </c>
+      <c r="B2428">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2429">
+        <v>11</v>
+      </c>
+      <c r="B2429">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2430">
+        <v>6</v>
+      </c>
+      <c r="B2430">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2431">
+        <v>15</v>
+      </c>
+      <c r="B2431">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2432">
+        <v>20</v>
+      </c>
+      <c r="B2432">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2433">
+        <v>3</v>
+      </c>
+      <c r="B2433">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2434">
+        <v>1</v>
+      </c>
+      <c r="B2434">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2435">
+        <v>16</v>
+      </c>
+      <c r="B2435">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2436">
+        <v>19</v>
+      </c>
+      <c r="B2436">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2437">
+        <v>6</v>
+      </c>
+      <c r="B2437">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2438">
+        <v>5</v>
+      </c>
+      <c r="B2438">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2439">
+        <v>13</v>
+      </c>
+      <c r="B2439">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2440">
+        <v>8</v>
+      </c>
+      <c r="B2440">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2441">
+        <v>1</v>
+      </c>
+      <c r="B2441">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2442">
+        <v>16</v>
+      </c>
+      <c r="B2442">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2443">
+        <v>12</v>
+      </c>
+      <c r="B2443">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2444">
+        <v>12</v>
+      </c>
+      <c r="B2444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2445">
+        <v>11</v>
+      </c>
+      <c r="B2445">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2446">
+        <v>9</v>
+      </c>
+      <c r="B2446">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2447">
+        <v>2</v>
+      </c>
+      <c r="B2447">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2448">
+        <v>9</v>
+      </c>
+      <c r="B2448">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2449">
+        <v>2</v>
+      </c>
+      <c r="B2449">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2450">
+        <v>12</v>
+      </c>
+      <c r="B2450">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2451">
+        <v>7</v>
+      </c>
+      <c r="B2451">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2452">
+        <v>7</v>
+      </c>
+      <c r="B2452">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2453">
+        <v>6</v>
+      </c>
+      <c r="B2453">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2454">
+        <v>20</v>
+      </c>
+      <c r="B2454">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2455">
+        <v>9</v>
+      </c>
+      <c r="B2455">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2456">
+        <v>9</v>
+      </c>
+      <c r="B2456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2457">
+        <v>17</v>
+      </c>
+      <c r="B2457">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2458">
+        <v>13</v>
+      </c>
+      <c r="B2458">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2459">
+        <v>13</v>
+      </c>
+      <c r="B2459">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2460">
+        <v>11</v>
+      </c>
+      <c r="B2460">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2461">
+        <v>11</v>
+      </c>
+      <c r="B2461">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2462">
+        <v>13</v>
+      </c>
+      <c r="B2462">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2463">
+        <v>2</v>
+      </c>
+      <c r="B2463">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2464">
+        <v>11</v>
+      </c>
+      <c r="B2464">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2465">
+        <v>3</v>
+      </c>
+      <c r="B2465">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2466">
+        <v>6</v>
+      </c>
+      <c r="B2466">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2467">
+        <v>6</v>
+      </c>
+      <c r="B2467">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2468">
+        <v>3</v>
+      </c>
+      <c r="B2468">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2469">
+        <v>19</v>
+      </c>
+      <c r="B2469">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2470">
+        <v>1</v>
+      </c>
+      <c r="B2470">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2471">
+        <v>15</v>
+      </c>
+      <c r="B2471">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2472">
+        <v>19</v>
+      </c>
+      <c r="B2472">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2473">
+        <v>4</v>
+      </c>
+      <c r="B2473">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2474">
+        <v>10</v>
+      </c>
+      <c r="B2474">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2475">
+        <v>7</v>
+      </c>
+      <c r="B2475">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2476">
+        <v>15</v>
+      </c>
+      <c r="B2476">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2477">
+        <v>16</v>
+      </c>
+      <c r="B2477">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2478">
+        <v>8</v>
+      </c>
+      <c r="B2478">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2479">
+        <v>20</v>
+      </c>
+      <c r="B2479">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2480">
+        <v>2</v>
+      </c>
+      <c r="B2480">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2481">
+        <v>12</v>
+      </c>
+      <c r="B2481">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2482">
+        <v>15</v>
+      </c>
+      <c r="B2482">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2483">
+        <v>2</v>
+      </c>
+      <c r="B2483">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2484">
+        <v>9</v>
+      </c>
+      <c r="B2484">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2485">
+        <v>11</v>
+      </c>
+      <c r="B2485">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2486">
+        <v>17</v>
+      </c>
+      <c r="B2486">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2487">
+        <v>9</v>
+      </c>
+      <c r="B2487">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2488">
+        <v>19</v>
+      </c>
+      <c r="B2488">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2489">
+        <v>17</v>
+      </c>
+      <c r="B2489">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2490">
+        <v>3</v>
+      </c>
+      <c r="B2490">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2491">
+        <v>5</v>
+      </c>
+      <c r="B2491">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2492">
+        <v>19</v>
+      </c>
+      <c r="B2492">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2493">
+        <v>18</v>
+      </c>
+      <c r="B2493">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2494">
+        <v>20</v>
+      </c>
+      <c r="B2494">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2495">
+        <v>9</v>
+      </c>
+      <c r="B2495">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2496">
+        <v>13</v>
+      </c>
+      <c r="B2496">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2497">
+        <v>15</v>
+      </c>
+      <c r="B2497">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2498">
+        <v>5</v>
+      </c>
+      <c r="B2498">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2499">
+        <v>14</v>
+      </c>
+      <c r="B2499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2500">
+        <v>8</v>
+      </c>
+      <c r="B2500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2501">
+        <v>5</v>
+      </c>
+      <c r="B2501">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2502">
+        <v>4</v>
+      </c>
+      <c r="B2502">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2503">
+        <v>10</v>
+      </c>
+      <c r="B2503">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2504">
+        <v>4</v>
+      </c>
+      <c r="B2504">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2505">
+        <v>3</v>
+      </c>
+      <c r="B2505">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2506">
+        <v>13</v>
+      </c>
+      <c r="B2506">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2507">
+        <v>13</v>
+      </c>
+      <c r="B2507">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2508">
+        <v>2</v>
+      </c>
+      <c r="B2508">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2509">
+        <v>18</v>
+      </c>
+      <c r="B2509">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2510">
+        <v>19</v>
+      </c>
+      <c r="B2510">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2511">
+        <v>3</v>
+      </c>
+      <c r="B2511">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2512">
+        <v>8</v>
+      </c>
+      <c r="B2512">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2513">
+        <v>19</v>
+      </c>
+      <c r="B2513">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2514">
+        <v>19</v>
+      </c>
+      <c r="B2514">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2515">
+        <v>14</v>
+      </c>
+      <c r="B2515">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2516">
+        <v>7</v>
+      </c>
+      <c r="B2516">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2517">
+        <v>3</v>
+      </c>
+      <c r="B2517">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2518">
+        <v>11</v>
+      </c>
+      <c r="B2518">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2519">
+        <v>16</v>
+      </c>
+      <c r="B2519">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2520">
+        <v>17</v>
+      </c>
+      <c r="B2520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2521">
+        <v>12</v>
+      </c>
+      <c r="B2521">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2522">
+        <v>8</v>
+      </c>
+      <c r="B2522">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2523">
+        <v>9</v>
+      </c>
+      <c r="B2523">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2524">
+        <v>11</v>
+      </c>
+      <c r="B2524">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2525">
+        <v>3</v>
+      </c>
+      <c r="B2525">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2526">
+        <v>7</v>
+      </c>
+      <c r="B2526">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2527">
+        <v>9</v>
+      </c>
+      <c r="B2527">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2528">
+        <v>7</v>
+      </c>
+      <c r="B2528">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2529">
+        <v>19</v>
+      </c>
+      <c r="B2529">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2530">
+        <v>11</v>
+      </c>
+      <c r="B2530">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2531">
+        <v>13</v>
+      </c>
+      <c r="B2531">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2532">
+        <v>20</v>
+      </c>
+      <c r="B2532">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2533">
+        <v>16</v>
+      </c>
+      <c r="B2533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2534">
+        <v>14</v>
+      </c>
+      <c r="B2534">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2535">
+        <v>11</v>
+      </c>
+      <c r="B2535">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2536">
+        <v>5</v>
+      </c>
+      <c r="B2536">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2537">
+        <v>11</v>
+      </c>
+      <c r="B2537">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2538">
+        <v>11</v>
+      </c>
+      <c r="B2538">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2539">
+        <v>4</v>
+      </c>
+      <c r="B2539">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2540">
+        <v>17</v>
+      </c>
+      <c r="B2540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2541">
+        <v>20</v>
+      </c>
+      <c r="B2541">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2542">
+        <v>11</v>
+      </c>
+      <c r="B2542">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2543">
+        <v>16</v>
+      </c>
+      <c r="B2543">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2544">
+        <v>14</v>
+      </c>
+      <c r="B2544">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2545">
+        <v>3</v>
+      </c>
+      <c r="B2545">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2546">
+        <v>1</v>
+      </c>
+      <c r="B2546">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2547">
+        <v>2</v>
+      </c>
+      <c r="B2547">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2548">
+        <v>15</v>
+      </c>
+      <c r="B2548">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2549">
+        <v>19</v>
+      </c>
+      <c r="B2549">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2550">
+        <v>18</v>
+      </c>
+      <c r="B2550">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2551">
+        <v>3</v>
+      </c>
+      <c r="B2551">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2552">
+        <v>19</v>
+      </c>
+      <c r="B2552">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2553">
+        <v>16</v>
+      </c>
+      <c r="B2553">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2554">
+        <v>20</v>
+      </c>
+      <c r="B2554">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2555">
+        <v>5</v>
+      </c>
+      <c r="B2555">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2556">
+        <v>19</v>
+      </c>
+      <c r="B2556">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2557">
+        <v>12</v>
+      </c>
+      <c r="B2557">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2558">
+        <v>6</v>
+      </c>
+      <c r="B2558">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2559">
+        <v>2</v>
+      </c>
+      <c r="B2559">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2560">
+        <v>19</v>
+      </c>
+      <c r="B2560">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2561">
+        <v>6</v>
+      </c>
+      <c r="B2561">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2562">
+        <v>8</v>
+      </c>
+      <c r="B2562">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2563">
+        <v>12</v>
+      </c>
+      <c r="B2563">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2564">
+        <v>15</v>
+      </c>
+      <c r="B2564">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2565">
+        <v>20</v>
+      </c>
+      <c r="B2565">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2566">
+        <v>1</v>
+      </c>
+      <c r="B2566">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2567">
+        <v>16</v>
+      </c>
+      <c r="B2567">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2568">
+        <v>14</v>
+      </c>
+      <c r="B2568">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2569">
+        <v>3</v>
+      </c>
+      <c r="B2569">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2570">
+        <v>12</v>
+      </c>
+      <c r="B2570">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2571">
+        <v>12</v>
+      </c>
+      <c r="B2571">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2572">
+        <v>17</v>
+      </c>
+      <c r="B2572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2573">
+        <v>7</v>
+      </c>
+      <c r="B2573">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2574">
+        <v>13</v>
+      </c>
+      <c r="B2574">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2575">
+        <v>10</v>
+      </c>
+      <c r="B2575">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2576">
+        <v>12</v>
+      </c>
+      <c r="B2576">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2577">
+        <v>7</v>
+      </c>
+      <c r="B2577">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2578">
+        <v>19</v>
+      </c>
+      <c r="B2578">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2579">
+        <v>2</v>
+      </c>
+      <c r="B2579">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2580">
+        <v>5</v>
+      </c>
+      <c r="B2580">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2581">
+        <v>12</v>
+      </c>
+      <c r="B2581">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2582">
+        <v>5</v>
+      </c>
+      <c r="B2582">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2583">
+        <v>8</v>
+      </c>
+      <c r="B2583">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2584">
+        <v>3</v>
+      </c>
+      <c r="B2584">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2585">
+        <v>19</v>
+      </c>
+      <c r="B2585">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2586">
+        <v>1</v>
+      </c>
+      <c r="B2586">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2587">
+        <v>12</v>
+      </c>
+      <c r="B2587">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2588">
+        <v>1</v>
+      </c>
+      <c r="B2588">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2589">
+        <v>4</v>
+      </c>
+      <c r="B2589">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2590">
+        <v>3</v>
+      </c>
+      <c r="B2590">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2591">
+        <v>7</v>
+      </c>
+      <c r="B2591">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2592">
+        <v>13</v>
+      </c>
+      <c r="B2592">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2593">
+        <v>14</v>
+      </c>
+      <c r="B2593">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2594">
+        <v>13</v>
+      </c>
+      <c r="B2594">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2595">
+        <v>7</v>
+      </c>
+      <c r="B2595">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2596">
+        <v>17</v>
+      </c>
+      <c r="B2596">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2597">
+        <v>10</v>
+      </c>
+      <c r="B2597">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2598">
+        <v>13</v>
+      </c>
+      <c r="B2598">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2599">
+        <v>14</v>
+      </c>
+      <c r="B2599">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2600">
+        <v>12</v>
+      </c>
+      <c r="B2600">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2601">
+        <v>5</v>
+      </c>
+      <c r="B2601">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2602">
+        <v>12</v>
+      </c>
+      <c r="B2602">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2603">
+        <v>13</v>
+      </c>
+      <c r="B2603">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2604">
+        <v>5</v>
+      </c>
+      <c r="B2604">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2605">
+        <v>7</v>
+      </c>
+      <c r="B2605">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2606">
+        <v>14</v>
+      </c>
+      <c r="B2606">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2607">
+        <v>17</v>
+      </c>
+      <c r="B2607">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2608">
+        <v>15</v>
+      </c>
+      <c r="B2608">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2609">
+        <v>16</v>
+      </c>
+      <c r="B2609">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2610">
+        <v>13</v>
+      </c>
+      <c r="B2610">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2611">
+        <v>11</v>
+      </c>
+      <c r="B2611">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2612">
+        <v>10</v>
+      </c>
+      <c r="B2612">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2613">
+        <v>3</v>
+      </c>
+      <c r="B2613">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2614">
+        <v>7</v>
+      </c>
+      <c r="B2614">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2615">
+        <v>16</v>
+      </c>
+      <c r="B2615">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2616">
+        <v>4</v>
+      </c>
+      <c r="B2616">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2617">
+        <v>10</v>
+      </c>
+      <c r="B2617">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2618">
+        <v>14</v>
+      </c>
+      <c r="B2618">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2619">
+        <v>3</v>
+      </c>
+      <c r="B2619">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2620">
+        <v>12</v>
+      </c>
+      <c r="B2620">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2621">
+        <v>3</v>
+      </c>
+      <c r="B2621">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2622">
+        <v>6</v>
+      </c>
+      <c r="B2622">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2623">
+        <v>19</v>
+      </c>
+      <c r="B2623">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2624">
+        <v>4</v>
+      </c>
+      <c r="B2624">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2625">
+        <v>8</v>
+      </c>
+      <c r="B2625">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2626">
+        <v>8</v>
+      </c>
+      <c r="B2626">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2627">
+        <v>11</v>
+      </c>
+      <c r="B2627">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2628">
+        <v>10</v>
+      </c>
+      <c r="B2628">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2629">
+        <v>15</v>
+      </c>
+      <c r="B2629">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2630">
+        <v>12</v>
+      </c>
+      <c r="B2630">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2631">
+        <v>2</v>
+      </c>
+      <c r="B2631">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2632">
+        <v>1</v>
+      </c>
+      <c r="B2632">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2633">
+        <v>7</v>
+      </c>
+      <c r="B2633">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2634">
+        <v>15</v>
+      </c>
+      <c r="B2634">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2635">
+        <v>14</v>
+      </c>
+      <c r="B2635">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2636">
+        <v>13</v>
+      </c>
+      <c r="B2636">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2637">
+        <v>19</v>
+      </c>
+      <c r="B2637">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2638">
+        <v>3</v>
+      </c>
+      <c r="B2638">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2639">
+        <v>10</v>
+      </c>
+      <c r="B2639">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2640">
+        <v>2</v>
+      </c>
+      <c r="B2640">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2641">
+        <v>1</v>
+      </c>
+      <c r="B2641">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2642">
+        <v>12</v>
+      </c>
+      <c r="B2642">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2643">
+        <v>15</v>
+      </c>
+      <c r="B2643">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2644">
+        <v>13</v>
+      </c>
+      <c r="B2644">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2645">
+        <v>8</v>
+      </c>
+      <c r="B2645">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2646">
+        <v>11</v>
+      </c>
+      <c r="B2646">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2647">
+        <v>3</v>
+      </c>
+      <c r="B2647">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2648">
+        <v>18</v>
+      </c>
+      <c r="B2648">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2649">
+        <v>13</v>
+      </c>
+      <c r="B2649">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2650">
+        <v>10</v>
+      </c>
+      <c r="B2650">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2651">
+        <v>8</v>
+      </c>
+      <c r="B2651">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2652">
+        <v>11</v>
+      </c>
+      <c r="B2652">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2653">
+        <v>16</v>
+      </c>
+      <c r="B2653">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2654">
+        <v>7</v>
+      </c>
+      <c r="B2654">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2655">
+        <v>3</v>
+      </c>
+      <c r="B2655">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2656">
+        <v>9</v>
+      </c>
+      <c r="B2656">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2657">
+        <v>16</v>
+      </c>
+      <c r="B2657">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2658">
+        <v>2</v>
+      </c>
+      <c r="B2658">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2659">
+        <v>18</v>
+      </c>
+      <c r="B2659">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2660">
+        <v>4</v>
+      </c>
+      <c r="B2660">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2661">
+        <v>8</v>
+      </c>
+      <c r="B2661">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2662">
+        <v>10</v>
+      </c>
+      <c r="B2662">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2663">
+        <v>19</v>
+      </c>
+      <c r="B2663">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2664">
+        <v>16</v>
+      </c>
+      <c r="B2664">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2665">
+        <v>11</v>
+      </c>
+      <c r="B2665">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2666">
+        <v>1</v>
+      </c>
+      <c r="B2666">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2667">
+        <v>14</v>
+      </c>
+      <c r="B2667">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2668">
+        <v>2</v>
+      </c>
+      <c r="B2668">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2669">
+        <v>4</v>
+      </c>
+      <c r="B2669">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2670">
+        <v>8</v>
+      </c>
+      <c r="B2670">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2671">
+        <v>3</v>
+      </c>
+      <c r="B2671">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2672">
+        <v>8</v>
+      </c>
+      <c r="B2672">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2673">
+        <v>2</v>
+      </c>
+      <c r="B2673">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2674">
+        <v>6</v>
+      </c>
+      <c r="B2674">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2675">
+        <v>3</v>
+      </c>
+      <c r="B2675">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2676">
+        <v>17</v>
+      </c>
+      <c r="B2676">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2677">
+        <v>7</v>
+      </c>
+      <c r="B2677">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2678">
+        <v>15</v>
+      </c>
+      <c r="B2678">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2679">
+        <v>13</v>
+      </c>
+      <c r="B2679">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2680">
+        <v>11</v>
+      </c>
+      <c r="B2680">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2681">
+        <v>16</v>
+      </c>
+      <c r="B2681">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2682">
+        <v>1</v>
+      </c>
+      <c r="B2682">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2683">
+        <v>13</v>
+      </c>
+      <c r="B2683">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2684">
+        <v>9</v>
+      </c>
+      <c r="B2684">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2685">
+        <v>18</v>
+      </c>
+      <c r="B2685">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2686">
+        <v>13</v>
+      </c>
+      <c r="B2686">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2687">
+        <v>15</v>
+      </c>
+      <c r="B2687">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2688">
+        <v>3</v>
+      </c>
+      <c r="B2688">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2689">
+        <v>1</v>
+      </c>
+      <c r="B2689">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2690">
+        <v>15</v>
+      </c>
+      <c r="B2690">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2691">
+        <v>18</v>
+      </c>
+      <c r="B2691">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2692">
+        <v>13</v>
+      </c>
+      <c r="B2692">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2693">
+        <v>2</v>
+      </c>
+      <c r="B2693">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2694">
+        <v>14</v>
+      </c>
+      <c r="B2694">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2695">
+        <v>6</v>
+      </c>
+      <c r="B2695">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2696">
+        <v>14</v>
+      </c>
+      <c r="B2696">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2697">
+        <v>8</v>
+      </c>
+      <c r="B2697">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2698">
+        <v>17</v>
+      </c>
+      <c r="B2698">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2699">
+        <v>10</v>
+      </c>
+      <c r="B2699">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2700">
+        <v>9</v>
+      </c>
+      <c r="B2700">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2701">
+        <v>12</v>
+      </c>
+      <c r="B2701">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2702">
+        <v>3</v>
+      </c>
+      <c r="B2702">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2703">
+        <v>9</v>
+      </c>
+      <c r="B2703">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2704">
+        <v>17</v>
+      </c>
+      <c r="B2704">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>